<commit_message>
format changed of 2 files dhan bahadur sth pahiro and indrayani mandir for giving it to sahadev sir
</commit_message>
<xml_diff>
--- a/ofc/estimates/2024-12-10 dhan bahadur sth ko paxadi pahiro/धन बहादुर श्रेष्ठको घर पछाडी पहिरो संरक्षण.xlsx
+++ b/ofc/estimates/2024-12-10 dhan bahadur sth ko paxadi pahiro/धन बहादुर श्रेष्ठको घर पछाडी पहिरो संरक्षण.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\2024-12-10 dhan bahadur sth ko paxadi pahiro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\2024-12-10 dhan bahadur sth ko paxadi pahiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -244,10 +244,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -439,7 +439,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -449,7 +449,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,14 +469,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,7 +485,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -509,7 +509,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,7 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -559,7 +559,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -575,11 +575,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1364,22 +1364,22 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="J1" s="61"/>
       <c r="K1" s="61"/>
     </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
         <v>1</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="J2" s="62"/>
       <c r="K2" s="62"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>2</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="J3" s="63"/>
       <c r="K3" s="63"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
@@ -1439,7 +1439,7 @@
       <c r="J4" s="63"/>
       <c r="K4" s="63"/>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="64" t="s">
         <v>18</v>
       </c>
@@ -1454,7 +1454,7 @@
       <c r="J5" s="64"/>
       <c r="K5" s="64"/>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="K6" s="60"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
@@ -1492,7 +1492,7 @@
       <c r="J7" s="69"/>
       <c r="K7" s="69"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1508,7 +1508,7 @@
       <c r="J8" s="70"/>
       <c r="K8" s="70"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="71" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1524,7 +1524,7 @@
       <c r="J9" s="70"/>
       <c r="K9" s="70"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>21</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="65"/>
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
@@ -1576,7 +1576,7 @@
       <c r="J12" s="65"/>
       <c r="K12" s="66"/>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="32" t="e">
         <f>#REF!</f>
@@ -1641,7 +1641,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="12"/>
@@ -1654,7 +1654,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="12"/>
@@ -1710,7 +1710,7 @@
       <c r="J17" s="27"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1773,25 +1773,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1806,7 @@
       <c r="J1" s="81"/>
       <c r="K1" s="81"/>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="J2" s="82"/>
       <c r="K2" s="82"/>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>2</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="J3" s="63"/>
       <c r="K3" s="63"/>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
@@ -1851,7 +1851,7 @@
       <c r="J4" s="63"/>
       <c r="K4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
@@ -1866,7 +1866,7 @@
       <c r="J5" s="83"/>
       <c r="K5" s="83"/>
     </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
         <v>58</v>
       </c>
@@ -1883,7 +1883,7 @@
       <c r="J6" s="80"/>
       <c r="K6" s="80"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>28</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="J7" s="75"/>
       <c r="K7" s="75"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
         <v>45</v>
@@ -1981,7 +1981,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="78"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="36" t="s">
         <v>41</v>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="K11" s="79"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="36"/>
       <c r="C12" s="19"/>
@@ -2019,7 +2019,7 @@
       <c r="J12" s="40"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:17" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>2</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="36" t="s">
         <v>51</v>
@@ -2073,7 +2073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="36" t="s">
         <v>41</v>
@@ -2113,7 +2113,7 @@
         <v>2754.6623333333332</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="36" t="s">
         <v>47</v>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="29"/>
       <c r="C17" s="19"/>
@@ -2144,7 +2144,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="36" t="s">
         <v>45</v>
@@ -2189,7 +2189,7 @@
       <c r="J19" s="39"/>
       <c r="K19" s="58"/>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="36"/>
       <c r="C20" s="35">
@@ -2213,7 +2213,7 @@
       <c r="J20" s="39"/>
       <c r="K20" s="58"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="36" t="s">
         <v>41</v>
@@ -2246,7 +2246,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
         <v>47</v>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="36"/>
       <c r="C23" s="19"/>
@@ -2277,7 +2277,7 @@
       <c r="J23" s="40"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>4</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="36" t="s">
         <v>49</v>
@@ -2320,7 +2320,7 @@
       <c r="J25" s="39"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="36" t="s">
         <v>41</v>
@@ -2353,7 +2353,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="36" t="s">
         <v>47</v>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="36"/>
       <c r="C28" s="19"/>
@@ -2384,7 +2384,7 @@
       <c r="J28" s="40"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>5</v>
       </c>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="24"/>
       <c r="C30" s="19"/>
@@ -2426,7 +2426,7 @@
       <c r="J30" s="40"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
       <c r="B31" s="41" t="s">
         <v>17</v>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="K31" s="35"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="53"/>
       <c r="B32" s="56"/>
       <c r="C32" s="57"/>
@@ -2457,7 +2457,7 @@
       <c r="J32" s="55"/>
       <c r="K32" s="52"/>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="45"/>
       <c r="B33" s="28" t="s">
         <v>27</v>
@@ -2477,7 +2477,7 @@
       <c r="J33" s="49"/>
       <c r="K33" s="50"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="51"/>
       <c r="B34" s="28" t="s">
         <v>32</v>
@@ -2494,7 +2494,7 @@
       <c r="J34" s="43"/>
       <c r="K34" s="44"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="51"/>
       <c r="B35" s="28" t="s">
         <v>33</v>
@@ -2515,7 +2515,7 @@
       <c r="J35" s="43"/>
       <c r="K35" s="44"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="51"/>
       <c r="B36" s="28" t="s">
         <v>34</v>
@@ -2536,7 +2536,7 @@
       <c r="J36" s="43"/>
       <c r="K36" s="44"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="51"/>
       <c r="B37" s="28" t="s">
         <v>35</v>
@@ -2556,7 +2556,7 @@
       <c r="J37" s="43"/>
       <c r="K37" s="44"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="51"/>
       <c r="B38" s="28" t="s">
         <v>36</v>
@@ -2576,7 +2576,7 @@
       <c r="J38" s="43"/>
       <c r="K38" s="44"/>
     </row>
-    <row r="39" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
@@ -2589,62 +2589,62 @@
       <c r="J39" s="52"/>
       <c r="K39" s="52"/>
     </row>
-    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="A6:F6"/>
@@ -2668,10 +2668,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
-Er. Prakash Singh Saud</oddFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>